<commit_message>
bonus gera + bonus M1
</commit_message>
<xml_diff>
--- a/polosaomiguel.xlsx
+++ b/polosaomiguel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b9c5cb4a62800de0/Desktop/RepoNOvo/pandastest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="159" documentId="8_{154E9F5E-6070-441A-966F-73CFEFA71421}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E462602C-F605-4138-BB58-3D8F5B62279E}"/>
+  <xr:revisionPtr revIDLastSave="173" documentId="8_{154E9F5E-6070-441A-966F-73CFEFA71421}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{54366299-BA8F-470D-935D-83D4A3BA542D}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{14D27C5C-7C50-498F-A52C-EE811162B8B5}"/>
   </bookViews>
@@ -38,9 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
   <si>
-    <t>executivos</t>
-  </si>
-  <si>
     <t>Marcela</t>
   </si>
   <si>
@@ -96,6 +93,9 @@
   </si>
   <si>
     <t>VIP</t>
+  </si>
+  <si>
+    <t>executivo</t>
   </si>
 </sst>
 </file>
@@ -477,52 +477,51 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="24.88671875" customWidth="1"/>
-    <col min="2" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="7" width="9" customWidth="1"/>
-    <col min="8" max="8" width="9.6640625" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" customWidth="1"/>
+    <col min="3" max="9" width="10.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="I1" t="s">
         <v>15</v>
-      </c>
-      <c r="F1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2">
         <v>9</v>
@@ -531,7 +530,7 @@
         <v>9</v>
       </c>
       <c r="E2">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="F2">
         <v>11</v>
@@ -544,15 +543,15 @@
       </c>
       <c r="I2">
         <f>SUM(C2:E2)*100</f>
-        <v>2000</v>
+        <v>2700</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C3">
         <v>8</v>
@@ -561,7 +560,7 @@
         <v>5</v>
       </c>
       <c r="E3">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F3">
         <v>18</v>
@@ -574,15 +573,15 @@
       </c>
       <c r="I3">
         <f t="shared" ref="I3:I10" si="0">SUM(C3:E3)*100</f>
-        <v>1700</v>
+        <v>2200</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -609,10 +608,10 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5">
         <v>6</v>
@@ -639,19 +638,19 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6">
+        <v>9</v>
+      </c>
+      <c r="D6">
+        <v>9</v>
+      </c>
+      <c r="E6">
         <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6">
-        <v>9</v>
-      </c>
-      <c r="D6">
-        <v>9</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
       </c>
       <c r="F6">
         <v>18</v>
@@ -664,15 +663,15 @@
       </c>
       <c r="I6">
         <f t="shared" si="0"/>
-        <v>1900</v>
+        <v>2300</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7">
         <v>3</v>
@@ -699,10 +698,10 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8">
         <v>9</v>
@@ -729,10 +728,10 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9">
         <v>6</v>
@@ -759,10 +758,10 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10">
         <v>5</v>

</xml_diff>